<commit_message>
perbaikan input praktik keperawatan profesi
</commit_message>
<xml_diff>
--- a/_file/praktik/data_praktikan_1_2022-03-12.xlsx
+++ b/_file/praktik/data_praktikan_1_2022-03-12.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fajar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fajar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="49">
   <si>
     <t>NO.</t>
   </si>
@@ -144,6 +144,42 @@
   </si>
   <si>
     <t>KOTA CIMAHI</t>
+  </si>
+  <si>
+    <t>SITHA RAMADHANI A.</t>
+  </si>
+  <si>
+    <t>087623918732</t>
+  </si>
+  <si>
+    <t>ramasd123@gmail.com</t>
+  </si>
+  <si>
+    <t>ARIF HAKIM</t>
+  </si>
+  <si>
+    <t>0822891238911</t>
+  </si>
+  <si>
+    <t>arif_hakim@gmail.com</t>
+  </si>
+  <si>
+    <t>ADI HARDIANSYAH</t>
+  </si>
+  <si>
+    <t>0889263223683</t>
+  </si>
+  <si>
+    <t>adihhardianr@gmail.com</t>
+  </si>
+  <si>
+    <t>KAB. BANDUNG BARAT</t>
+  </si>
+  <si>
+    <t>NANDANG</t>
+  </si>
+  <si>
+    <t>nandang@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -634,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1262,6 +1298,122 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1010202208</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1010202209</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1010202210</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1010202211</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G1">
     <sortState ref="A2:G44">
@@ -1270,15 +1422,19 @@
   </autoFilter>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3:F8" r:id="rId2" display="adeamr@gmail.com"/>
+    <hyperlink ref="F3:F12" r:id="rId2" display="adeamr@gmail.com"/>
     <hyperlink ref="F3" r:id="rId3"/>
     <hyperlink ref="F4" r:id="rId4"/>
     <hyperlink ref="F5" r:id="rId5"/>
     <hyperlink ref="F6" r:id="rId6"/>
     <hyperlink ref="F7" r:id="rId7"/>
     <hyperlink ref="F8" r:id="rId8"/>
+    <hyperlink ref="F9" r:id="rId9"/>
+    <hyperlink ref="F10" r:id="rId10"/>
+    <hyperlink ref="F11" r:id="rId11"/>
+    <hyperlink ref="F12" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>